<commit_message>
Last Update PCB Kevin
</commit_message>
<xml_diff>
--- a/Electronic/PCB/Motor Driver/Motor Driver/Project Outputs for Motor Driver/BOM/Bill of Materials-Motor Driver.xlsx
+++ b/Electronic/PCB/Motor Driver/Motor Driver/Project Outputs for Motor Driver/BOM/Bill of Materials-Motor Driver.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukab\Desktop\DEC\6DOF-Robotic-Arm\Electronic\PCB\Motor Driver\Motor Driver\Project Outputs for Motor Driver\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emile\6DOF-Robotic-Arm\Electronic\PCB\Motor Driver\Motor Driver\Project Outputs for Motor Driver\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AD09C39-F2DF-41FF-8B1C-953E641A0FEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="840" windowWidth="21600" windowHeight="11130" xr2:uid="{84A200C9-4E13-447D-95CC-8AFC638DE52A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Motor Driver" sheetId="1" r:id="rId1"/>
@@ -18,16 +17,10 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Bill of Materials-Motor Driver'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -408,10 +401,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -489,7 +482,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -505,7 +498,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -517,7 +510,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -564,23 +557,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -616,23 +592,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -784,7 +743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36C5454-4677-4F22-8681-BF7FD8A48D12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -792,9 +751,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="6" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -817,7 +776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -837,7 +796,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -857,7 +816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -877,7 +836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -897,7 +856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -1017,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
@@ -1077,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>56</v>
       </c>
@@ -1097,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>59</v>
       </c>
@@ -1117,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>62</v>
       </c>
@@ -1137,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>65</v>
       </c>
@@ -1157,7 +1116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>67</v>
       </c>
@@ -1177,7 +1136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>70</v>
       </c>
@@ -1197,7 +1156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>73</v>
       </c>
@@ -1217,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>76</v>
       </c>
@@ -1237,7 +1196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -1257,7 +1216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>82</v>
       </c>
@@ -1297,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>89</v>
       </c>
@@ -1317,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>94</v>
       </c>
@@ -1337,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>99</v>
       </c>
@@ -1357,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>104</v>
       </c>
@@ -1397,7 +1356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>113</v>
       </c>
@@ -1440,6 +1399,6 @@
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="70" orientation="landscape" blackAndWhite="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="64" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>